<commit_message>
endnote time for wos and proquest
</commit_message>
<xml_diff>
--- a/scripts/Common Alloys' Names.xlsx
+++ b/scripts/Common Alloys' Names.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="267">
   <si>
     <t xml:space="preserve">Aluminum</t>
   </si>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">        Bell metal (tin)</t>
   </si>
   <si>
-    <t xml:space="preserve">        Florentine bronze (aluminum or tin)</t>
+    <t xml:space="preserve">        Florentine bronze (aluminum, tin)</t>
   </si>
   <si>
     <t xml:space="preserve">        Glucydur (beryllium, iron)</t>
@@ -376,9 +376,6 @@
     <t xml:space="preserve">carbon steel (carbon)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ferrous alloys</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Elinvar (nickel, chromium)</t>
   </si>
   <si>
@@ -442,7 +439,7 @@
     <t xml:space="preserve">    Spiegeleisen (manganese, carbon, silicon)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Staballoy (managanese, chromium, carbon) </t>
+    <t xml:space="preserve">    Staballoy (manganese, chromium, carbon) </t>
   </si>
   <si>
     <t xml:space="preserve">        Bulat steel (carbon)</t>
@@ -508,7 +505,7 @@
     <t xml:space="preserve">            Zeron 100 (chromium, nickel, molybdenum)</t>
   </si>
   <si>
-    <t xml:space="preserve">        Tool steel (tungsten or manganese)</t>
+    <t xml:space="preserve">        Tool steel (tungsten, manganese)</t>
   </si>
   <si>
     <t xml:space="preserve">            Silver steel (manganese, chromium, silicon)</t>
@@ -577,7 +574,7 @@
     <t xml:space="preserve">    Chromel (chromium)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Cupronickel (bronze, copper)</t>
+    <t xml:space="preserve">    Cupronickel (tin, copper)</t>
   </si>
   <si>
     <t xml:space="preserve">    Ferronickel (iron)</t>
@@ -613,7 +610,7 @@
     <t xml:space="preserve">    Nisil (silicon)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Nitinol (titanium, shape memory alloy)</t>
+    <t xml:space="preserve">    Nitinol (titanium)</t>
   </si>
   <si>
     <t xml:space="preserve">        Mu-metal (iron)</t>
@@ -682,7 +679,7 @@
     <t xml:space="preserve">    Mischmetal (cerium, lanthanum, neodymium)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Terfenol-D (terbium, dysprosium, and iron) </t>
+    <t xml:space="preserve">    Terfenol-D (terbium, dysprosium, iron) </t>
   </si>
   <si>
     <t xml:space="preserve">    Ferrocerium (cerium, iron)</t>
@@ -754,7 +751,7 @@
     <t xml:space="preserve">    6al–4v (aluminum, vanadium)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Beta C (vanadium, chromium, others)</t>
+    <t xml:space="preserve">    Beta C (vanadium, chromium)</t>
   </si>
   <si>
     <t xml:space="preserve">    Gum metal (niobium, tantalum, zirconium, oxygen) </t>
@@ -781,7 +778,7 @@
     <t xml:space="preserve">    Pewter (antimony, copper)</t>
   </si>
   <si>
-    <t xml:space="preserve">    Queen's metal (antimony, lead, and bismuth)</t>
+    <t xml:space="preserve">    Queen's metal (antimony, lead, bismuth)</t>
   </si>
   <si>
     <t xml:space="preserve">    Solder (lead, antimony)</t>
@@ -790,7 +787,7 @@
     <t xml:space="preserve">    Terne (lead)</t>
   </si>
   <si>
-    <t xml:space="preserve">    White metal (copper or lead) </t>
+    <t xml:space="preserve">    White metal (copper, lead) </t>
   </si>
   <si>
     <t xml:space="preserve">Uranium</t>
@@ -927,8 +924,8 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A221" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P229" activeCellId="0" sqref="P229"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A294" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A295" activeCellId="0" sqref="A295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1865,12 +1862,12 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>165</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>2</v>
+        <v>165</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,12 +1877,12 @@
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>167</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>2</v>
+        <v>167</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,12 +1902,12 @@
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>171</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>2</v>
+        <v>171</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,12 +1917,12 @@
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>173</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>2</v>
+        <v>173</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,12 +1932,12 @@
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>175</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>2</v>
+        <v>175</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,12 +1947,12 @@
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>177</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>2</v>
+        <v>177</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,12 +1962,12 @@
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>179</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>2</v>
+        <v>179</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,12 +1977,12 @@
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>181</v>
+        <v>2</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>2</v>
+        <v>181</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,12 +2097,12 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>204</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>2</v>
+        <v>204</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,12 +2112,12 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>206</v>
+        <v>2</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>2</v>
+        <v>206</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2150,12 +2147,12 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>212</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2165,12 +2162,12 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>214</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>2</v>
+        <v>214</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,12 +2177,12 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>216</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>2</v>
+        <v>216</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,12 +2192,12 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>218</v>
+        <v>2</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>2</v>
+        <v>218</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,17 +2212,17 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>221</v>
+        <v>2</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>2</v>
+        <v>221</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>222</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,22 +2232,22 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>2</v>
+        <v>222</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>223</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>2</v>
+        <v>223</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>224</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2260,22 +2257,22 @@
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>2</v>
+        <v>224</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>225</v>
+        <v>2</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>2</v>
+        <v>225</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,17 +2282,17 @@
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>2</v>
+        <v>226</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>227</v>
+        <v>2</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>2</v>
+        <v>227</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,12 +2302,12 @@
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>229</v>
+        <v>2</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>2</v>
+        <v>229</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,17 +2352,17 @@
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>238</v>
+        <v>2</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>2</v>
+        <v>238</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>239</v>
+        <v>2</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,17 +2372,17 @@
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>2</v>
+        <v>239</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>240</v>
+        <v>2</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>2</v>
+        <v>240</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2395,12 +2392,12 @@
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>242</v>
+        <v>2</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>2</v>
+        <v>242</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,27 +2427,27 @@
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>248</v>
+        <v>2</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>26</v>
+        <v>248</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>249</v>
+        <v>2</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>2</v>
+        <v>249</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,12 +2482,12 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
-        <v>256</v>
+        <v>2</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="s">
-        <v>2</v>
+        <v>256</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,12 +2497,12 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="s">
-        <v>258</v>
+        <v>2</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="s">
-        <v>2</v>
+        <v>258</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2515,12 +2512,12 @@
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="s">
-        <v>260</v>
+        <v>2</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="s">
-        <v>2</v>
+        <v>260</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2530,27 +2527,27 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
-        <v>262</v>
+        <v>2</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="s">
-        <v>263</v>
+        <v>2</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="s">
-        <v>2</v>
+        <v>263</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="s">
-        <v>264</v>
+        <v>2</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2558,24 +2555,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="s">
-        <v>2</v>
+        <v>264</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="s">
-        <v>265</v>
+        <v>2</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
-        <v>2</v>
+        <v>265</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="s">
-        <v>266</v>
+        <v>2</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,14 +2582,10 @@
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>